<commit_message>
modified:   Mortgage Calc Final Boss Excel output.py 	modified:   Mortgage_results_1.xlsx
</commit_message>
<xml_diff>
--- a/Mortgage_results_1.xlsx
+++ b/Mortgage_results_1.xlsx
@@ -13,9 +13,59 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Loan Term (Years)</t>
+  </si>
+  <si>
+    <t>Interest Rate</t>
+  </si>
+  <si>
+    <t>Down Payment %</t>
+  </si>
+  <si>
+    <t>Monthly Payment</t>
+  </si>
+  <si>
+    <t>Total Interest Paid</t>
+  </si>
+  <si>
+    <t>Total Paid Over Life</t>
+  </si>
+  <si>
+    <t>Principal Paid by Year 4</t>
+  </si>
+  <si>
+    <t>Interest Paid by Year 4</t>
+  </si>
+  <si>
+    <t>Total Payment by Year 4</t>
+  </si>
+  <si>
+    <t>Principal Remaining after Year 4</t>
+  </si>
+  <si>
+    <t>Principal Paid by Year 5</t>
+  </si>
+  <si>
+    <t>Interest Paid by Year 5</t>
+  </si>
+  <si>
+    <t>Total Payment by Year 5</t>
+  </si>
+  <si>
+    <t>Principal Remaining after Year 5</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +73,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +104,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +421,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1500.558277245946</v>
+      </c>
+      <c r="E2" s="2">
+        <v>89160.78384684032</v>
+      </c>
+      <c r="F2" s="2">
+        <v>439160.7838468325</v>
+      </c>
+      <c r="G2" s="2">
+        <v>46378.59081439151</v>
+      </c>
+      <c r="H2" s="2">
+        <v>25648.20649341391</v>
+      </c>
+      <c r="I2" s="2">
+        <v>72026.79730780542</v>
+      </c>
+      <c r="J2" s="2">
+        <v>296621.4091856085</v>
+      </c>
+      <c r="K2" s="2">
+        <v>58564.1599818929</v>
+      </c>
+      <c r="L2" s="2">
+        <v>31469.33665286388</v>
+      </c>
+      <c r="M2" s="2">
+        <v>90033.49663475677</v>
+      </c>
+      <c r="N2" s="2">
+        <v>284435.8400181071</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>